<commit_message>
cleaned useless stuff from mpi_main.c
</commit_message>
<xml_diff>
--- a/apdGraphsAssignment2.xlsx
+++ b/apdGraphsAssignment2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\silver\code\apd\epidemic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5DEAE69-1D78-4256-93BC-5D6F9A5C42A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{959F619B-B613-4F9A-BF15-420A654902DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,10 +17,6 @@
     <sheet name="parallel_v1" sheetId="7" r:id="rId2"/>
     <sheet name="parallel_v2" sheetId="6" r:id="rId3"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId4"/>
-    <externalReference r:id="rId5"/>
-  </externalReferences>
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="2" hidden="1">parallel_v2!$A$1:$F$226</definedName>
     <definedName name="ExternalData_2" localSheetId="1" hidden="1">parallel_v1!$A$1:$D$451</definedName>
@@ -8702,1839 +8698,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="results"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="2">
-          <cell r="C2">
-            <v>2</v>
-          </cell>
-          <cell r="F2">
-            <v>0.82344099999999998</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="C3">
-            <v>3</v>
-          </cell>
-          <cell r="F3">
-            <v>0.88662200000000002</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="C4">
-            <v>4</v>
-          </cell>
-          <cell r="F4">
-            <v>0.71509299999999998</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="C5">
-            <v>5</v>
-          </cell>
-          <cell r="F5">
-            <v>0.67049800000000004</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="C6">
-            <v>6</v>
-          </cell>
-          <cell r="F6">
-            <v>0.732514</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="C7">
-            <v>7</v>
-          </cell>
-          <cell r="F7">
-            <v>0.61194599999999999</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="C8">
-            <v>8</v>
-          </cell>
-          <cell r="F8">
-            <v>0.65296799999999999</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="C9">
-            <v>9</v>
-          </cell>
-          <cell r="F9">
-            <v>0.52578199999999997</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="C10">
-            <v>10</v>
-          </cell>
-          <cell r="F10">
-            <v>0.55574000000000001</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="C11">
-            <v>2</v>
-          </cell>
-          <cell r="F11">
-            <v>0.85761200000000004</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="C12">
-            <v>3</v>
-          </cell>
-          <cell r="F12">
-            <v>1.3038069999999999</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="C13">
-            <v>4</v>
-          </cell>
-          <cell r="F13">
-            <v>0.93574900000000005</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="C14">
-            <v>5</v>
-          </cell>
-          <cell r="F14">
-            <v>0.65045500000000001</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="C15">
-            <v>6</v>
-          </cell>
-          <cell r="F15">
-            <v>0.71429600000000004</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="C16">
-            <v>7</v>
-          </cell>
-          <cell r="F16">
-            <v>0.63127800000000001</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="C17">
-            <v>8</v>
-          </cell>
-          <cell r="F17">
-            <v>0.60915399999999997</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="C18">
-            <v>9</v>
-          </cell>
-          <cell r="F18">
-            <v>0.55774199999999996</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="C19">
-            <v>10</v>
-          </cell>
-          <cell r="F19">
-            <v>0.55146499999999998</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="C20">
-            <v>2</v>
-          </cell>
-          <cell r="F20">
-            <v>1.019415</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="C21">
-            <v>3</v>
-          </cell>
-          <cell r="F21">
-            <v>1.4054489999999999</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="C22">
-            <v>4</v>
-          </cell>
-          <cell r="F22">
-            <v>0.82633299999999998</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="C23">
-            <v>5</v>
-          </cell>
-          <cell r="F23">
-            <v>0.83483399999999996</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="C24">
-            <v>6</v>
-          </cell>
-          <cell r="F24">
-            <v>0.77613200000000004</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="C25">
-            <v>7</v>
-          </cell>
-          <cell r="F25">
-            <v>0.66261899999999996</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="C26">
-            <v>8</v>
-          </cell>
-          <cell r="F26">
-            <v>0.57746600000000003</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="C27">
-            <v>9</v>
-          </cell>
-          <cell r="F27">
-            <v>0.52248000000000006</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="C28">
-            <v>10</v>
-          </cell>
-          <cell r="F28">
-            <v>0.41268500000000002</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="C29">
-            <v>2</v>
-          </cell>
-          <cell r="F29">
-            <v>1.002432</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="C30">
-            <v>3</v>
-          </cell>
-          <cell r="F30">
-            <v>1.1436839999999999</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="C31">
-            <v>4</v>
-          </cell>
-          <cell r="F31">
-            <v>1.1087549999999999</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="C32">
-            <v>5</v>
-          </cell>
-          <cell r="F32">
-            <v>0.838889</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="C33">
-            <v>6</v>
-          </cell>
-          <cell r="F33">
-            <v>0.68988799999999995</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="C34">
-            <v>7</v>
-          </cell>
-          <cell r="F34">
-            <v>0.76617800000000003</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="C35">
-            <v>8</v>
-          </cell>
-          <cell r="F35">
-            <v>0.62617400000000001</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="C36">
-            <v>9</v>
-          </cell>
-          <cell r="F36">
-            <v>0.59271799999999997</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="C37">
-            <v>10</v>
-          </cell>
-          <cell r="F37">
-            <v>0.59174800000000005</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="C38">
-            <v>2</v>
-          </cell>
-          <cell r="F38">
-            <v>1.2885230000000001</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="C39">
-            <v>3</v>
-          </cell>
-          <cell r="F39">
-            <v>1.3513790000000001</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="C40">
-            <v>4</v>
-          </cell>
-          <cell r="F40">
-            <v>1.3691530000000001</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="C41">
-            <v>5</v>
-          </cell>
-          <cell r="F41">
-            <v>0.90383100000000005</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="C42">
-            <v>6</v>
-          </cell>
-          <cell r="F42">
-            <v>0.88315299999999997</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="C43">
-            <v>7</v>
-          </cell>
-          <cell r="F43">
-            <v>0.73811400000000005</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="C44">
-            <v>8</v>
-          </cell>
-          <cell r="F44">
-            <v>0.68932499999999997</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="C45">
-            <v>9</v>
-          </cell>
-          <cell r="F45">
-            <v>0.64170300000000002</v>
-          </cell>
-        </row>
-        <row r="46">
-          <cell r="C46">
-            <v>10</v>
-          </cell>
-          <cell r="F46">
-            <v>0.63768000000000002</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="C47">
-            <v>2</v>
-          </cell>
-          <cell r="F47">
-            <v>1.04078</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="C48">
-            <v>3</v>
-          </cell>
-          <cell r="F48">
-            <v>1.0190410000000001</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="C49">
-            <v>4</v>
-          </cell>
-          <cell r="F49">
-            <v>1.068651</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="C50">
-            <v>5</v>
-          </cell>
-          <cell r="F50">
-            <v>1.0123789999999999</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="C51">
-            <v>6</v>
-          </cell>
-          <cell r="F51">
-            <v>1.123327</v>
-          </cell>
-        </row>
-        <row r="52">
-          <cell r="C52">
-            <v>7</v>
-          </cell>
-          <cell r="F52">
-            <v>1.0210079999999999</v>
-          </cell>
-        </row>
-        <row r="53">
-          <cell r="C53">
-            <v>8</v>
-          </cell>
-          <cell r="F53">
-            <v>0.97571099999999999</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="C54">
-            <v>9</v>
-          </cell>
-          <cell r="F54">
-            <v>0.93854599999999999</v>
-          </cell>
-        </row>
-        <row r="55">
-          <cell r="C55">
-            <v>10</v>
-          </cell>
-          <cell r="F55">
-            <v>0.92507300000000003</v>
-          </cell>
-        </row>
-        <row r="56">
-          <cell r="C56">
-            <v>2</v>
-          </cell>
-          <cell r="F56">
-            <v>1.04051</v>
-          </cell>
-        </row>
-        <row r="57">
-          <cell r="C57">
-            <v>3</v>
-          </cell>
-          <cell r="F57">
-            <v>1.1346510000000001</v>
-          </cell>
-        </row>
-        <row r="58">
-          <cell r="C58">
-            <v>4</v>
-          </cell>
-          <cell r="F58">
-            <v>1.473007</v>
-          </cell>
-        </row>
-        <row r="59">
-          <cell r="C59">
-            <v>5</v>
-          </cell>
-          <cell r="F59">
-            <v>1.2698579999999999</v>
-          </cell>
-        </row>
-        <row r="60">
-          <cell r="C60">
-            <v>6</v>
-          </cell>
-          <cell r="F60">
-            <v>1.2194799999999999</v>
-          </cell>
-        </row>
-        <row r="61">
-          <cell r="C61">
-            <v>7</v>
-          </cell>
-          <cell r="F61">
-            <v>1.089755</v>
-          </cell>
-        </row>
-        <row r="62">
-          <cell r="C62">
-            <v>8</v>
-          </cell>
-          <cell r="F62">
-            <v>1.0328079999999999</v>
-          </cell>
-        </row>
-        <row r="63">
-          <cell r="C63">
-            <v>9</v>
-          </cell>
-          <cell r="F63">
-            <v>0.91026700000000005</v>
-          </cell>
-        </row>
-        <row r="64">
-          <cell r="C64">
-            <v>10</v>
-          </cell>
-          <cell r="F64">
-            <v>1.039113</v>
-          </cell>
-        </row>
-        <row r="65">
-          <cell r="C65">
-            <v>2</v>
-          </cell>
-          <cell r="F65">
-            <v>1.1896230000000001</v>
-          </cell>
-        </row>
-        <row r="66">
-          <cell r="C66">
-            <v>3</v>
-          </cell>
-          <cell r="F66">
-            <v>1.3354569999999999</v>
-          </cell>
-        </row>
-        <row r="67">
-          <cell r="C67">
-            <v>4</v>
-          </cell>
-          <cell r="F67">
-            <v>1.458728</v>
-          </cell>
-        </row>
-        <row r="68">
-          <cell r="C68">
-            <v>5</v>
-          </cell>
-          <cell r="F68">
-            <v>1.30175</v>
-          </cell>
-        </row>
-        <row r="69">
-          <cell r="C69">
-            <v>6</v>
-          </cell>
-          <cell r="F69">
-            <v>1.2564660000000001</v>
-          </cell>
-        </row>
-        <row r="70">
-          <cell r="C70">
-            <v>7</v>
-          </cell>
-          <cell r="F70">
-            <v>1.1428739999999999</v>
-          </cell>
-        </row>
-        <row r="71">
-          <cell r="C71">
-            <v>8</v>
-          </cell>
-          <cell r="F71">
-            <v>1.06555</v>
-          </cell>
-        </row>
-        <row r="72">
-          <cell r="C72">
-            <v>9</v>
-          </cell>
-          <cell r="F72">
-            <v>0.82698799999999995</v>
-          </cell>
-        </row>
-        <row r="73">
-          <cell r="C73">
-            <v>10</v>
-          </cell>
-          <cell r="F73">
-            <v>0.924535</v>
-          </cell>
-        </row>
-        <row r="74">
-          <cell r="C74">
-            <v>2</v>
-          </cell>
-          <cell r="F74">
-            <v>1.1004719999999999</v>
-          </cell>
-        </row>
-        <row r="75">
-          <cell r="C75">
-            <v>3</v>
-          </cell>
-          <cell r="F75">
-            <v>1.766203</v>
-          </cell>
-        </row>
-        <row r="76">
-          <cell r="C76">
-            <v>4</v>
-          </cell>
-          <cell r="F76">
-            <v>1.6351899999999999</v>
-          </cell>
-        </row>
-        <row r="77">
-          <cell r="C77">
-            <v>5</v>
-          </cell>
-          <cell r="F77">
-            <v>1.3683069999999999</v>
-          </cell>
-        </row>
-        <row r="78">
-          <cell r="C78">
-            <v>6</v>
-          </cell>
-          <cell r="F78">
-            <v>1.393451</v>
-          </cell>
-        </row>
-        <row r="79">
-          <cell r="C79">
-            <v>7</v>
-          </cell>
-          <cell r="F79">
-            <v>1.2931060000000001</v>
-          </cell>
-        </row>
-        <row r="80">
-          <cell r="C80">
-            <v>8</v>
-          </cell>
-          <cell r="F80">
-            <v>1.187818</v>
-          </cell>
-        </row>
-        <row r="81">
-          <cell r="C81">
-            <v>9</v>
-          </cell>
-          <cell r="F81">
-            <v>1.234647</v>
-          </cell>
-        </row>
-        <row r="82">
-          <cell r="C82">
-            <v>10</v>
-          </cell>
-          <cell r="F82">
-            <v>1.0706260000000001</v>
-          </cell>
-        </row>
-        <row r="83">
-          <cell r="C83">
-            <v>2</v>
-          </cell>
-          <cell r="F83">
-            <v>1.2855829999999999</v>
-          </cell>
-        </row>
-        <row r="84">
-          <cell r="C84">
-            <v>3</v>
-          </cell>
-          <cell r="F84">
-            <v>1.349105</v>
-          </cell>
-        </row>
-        <row r="85">
-          <cell r="C85">
-            <v>4</v>
-          </cell>
-          <cell r="F85">
-            <v>1.513884</v>
-          </cell>
-        </row>
-        <row r="86">
-          <cell r="C86">
-            <v>5</v>
-          </cell>
-          <cell r="F86">
-            <v>1.431109</v>
-          </cell>
-        </row>
-        <row r="87">
-          <cell r="C87">
-            <v>6</v>
-          </cell>
-          <cell r="F87">
-            <v>1.438269</v>
-          </cell>
-        </row>
-        <row r="88">
-          <cell r="C88">
-            <v>7</v>
-          </cell>
-          <cell r="F88">
-            <v>1.21669</v>
-          </cell>
-        </row>
-        <row r="89">
-          <cell r="C89">
-            <v>8</v>
-          </cell>
-          <cell r="F89">
-            <v>1.2729269999999999</v>
-          </cell>
-        </row>
-        <row r="90">
-          <cell r="C90">
-            <v>9</v>
-          </cell>
-          <cell r="F90">
-            <v>1.257725</v>
-          </cell>
-        </row>
-        <row r="91">
-          <cell r="C91">
-            <v>10</v>
-          </cell>
-          <cell r="F91">
-            <v>1.0610649999999999</v>
-          </cell>
-        </row>
-        <row r="92">
-          <cell r="C92">
-            <v>2</v>
-          </cell>
-          <cell r="F92">
-            <v>1.30379</v>
-          </cell>
-        </row>
-        <row r="93">
-          <cell r="C93">
-            <v>3</v>
-          </cell>
-          <cell r="F93">
-            <v>1.737762</v>
-          </cell>
-        </row>
-        <row r="94">
-          <cell r="C94">
-            <v>4</v>
-          </cell>
-          <cell r="F94">
-            <v>1.914272</v>
-          </cell>
-        </row>
-        <row r="95">
-          <cell r="C95">
-            <v>5</v>
-          </cell>
-          <cell r="F95">
-            <v>1.839156</v>
-          </cell>
-        </row>
-        <row r="96">
-          <cell r="C96">
-            <v>6</v>
-          </cell>
-          <cell r="F96">
-            <v>1.567456</v>
-          </cell>
-        </row>
-        <row r="97">
-          <cell r="C97">
-            <v>7</v>
-          </cell>
-          <cell r="F97">
-            <v>1.750923</v>
-          </cell>
-        </row>
-        <row r="98">
-          <cell r="C98">
-            <v>8</v>
-          </cell>
-          <cell r="F98">
-            <v>1.737066</v>
-          </cell>
-        </row>
-        <row r="99">
-          <cell r="C99">
-            <v>9</v>
-          </cell>
-          <cell r="F99">
-            <v>1.9000699999999999</v>
-          </cell>
-        </row>
-        <row r="100">
-          <cell r="C100">
-            <v>10</v>
-          </cell>
-          <cell r="F100">
-            <v>1.8881950000000001</v>
-          </cell>
-        </row>
-        <row r="101">
-          <cell r="C101">
-            <v>2</v>
-          </cell>
-          <cell r="F101">
-            <v>1.4137949999999999</v>
-          </cell>
-        </row>
-        <row r="102">
-          <cell r="C102">
-            <v>3</v>
-          </cell>
-          <cell r="F102">
-            <v>1.650517</v>
-          </cell>
-        </row>
-        <row r="103">
-          <cell r="C103">
-            <v>4</v>
-          </cell>
-          <cell r="F103">
-            <v>1.771333</v>
-          </cell>
-        </row>
-        <row r="104">
-          <cell r="C104">
-            <v>5</v>
-          </cell>
-          <cell r="F104">
-            <v>1.841151</v>
-          </cell>
-        </row>
-        <row r="105">
-          <cell r="C105">
-            <v>6</v>
-          </cell>
-          <cell r="F105">
-            <v>1.802894</v>
-          </cell>
-        </row>
-        <row r="106">
-          <cell r="C106">
-            <v>7</v>
-          </cell>
-          <cell r="F106">
-            <v>1.99013</v>
-          </cell>
-        </row>
-        <row r="107">
-          <cell r="C107">
-            <v>8</v>
-          </cell>
-          <cell r="F107">
-            <v>2.0608580000000001</v>
-          </cell>
-        </row>
-        <row r="108">
-          <cell r="C108">
-            <v>9</v>
-          </cell>
-          <cell r="F108">
-            <v>2.2128589999999999</v>
-          </cell>
-        </row>
-        <row r="109">
-          <cell r="C109">
-            <v>10</v>
-          </cell>
-          <cell r="F109">
-            <v>2.0632630000000001</v>
-          </cell>
-        </row>
-        <row r="110">
-          <cell r="C110">
-            <v>2</v>
-          </cell>
-          <cell r="F110">
-            <v>1.553755</v>
-          </cell>
-        </row>
-        <row r="111">
-          <cell r="C111">
-            <v>3</v>
-          </cell>
-          <cell r="F111">
-            <v>1.756637</v>
-          </cell>
-        </row>
-        <row r="112">
-          <cell r="C112">
-            <v>4</v>
-          </cell>
-          <cell r="F112">
-            <v>1.9176420000000001</v>
-          </cell>
-        </row>
-        <row r="113">
-          <cell r="C113">
-            <v>5</v>
-          </cell>
-          <cell r="F113">
-            <v>1.9282410000000001</v>
-          </cell>
-        </row>
-        <row r="114">
-          <cell r="C114">
-            <v>6</v>
-          </cell>
-          <cell r="F114">
-            <v>1.916126</v>
-          </cell>
-        </row>
-        <row r="115">
-          <cell r="C115">
-            <v>7</v>
-          </cell>
-          <cell r="F115">
-            <v>2.0321829999999999</v>
-          </cell>
-        </row>
-        <row r="116">
-          <cell r="C116">
-            <v>8</v>
-          </cell>
-          <cell r="F116">
-            <v>2.116247</v>
-          </cell>
-        </row>
-        <row r="117">
-          <cell r="C117">
-            <v>9</v>
-          </cell>
-          <cell r="F117">
-            <v>2.1724389999999998</v>
-          </cell>
-        </row>
-        <row r="118">
-          <cell r="C118">
-            <v>10</v>
-          </cell>
-          <cell r="F118">
-            <v>2.1868300000000001</v>
-          </cell>
-        </row>
-        <row r="119">
-          <cell r="C119">
-            <v>2</v>
-          </cell>
-          <cell r="F119">
-            <v>1.542451</v>
-          </cell>
-        </row>
-        <row r="120">
-          <cell r="C120">
-            <v>3</v>
-          </cell>
-          <cell r="F120">
-            <v>1.813652</v>
-          </cell>
-        </row>
-        <row r="121">
-          <cell r="C121">
-            <v>4</v>
-          </cell>
-          <cell r="F121">
-            <v>2.044654</v>
-          </cell>
-        </row>
-        <row r="122">
-          <cell r="C122">
-            <v>5</v>
-          </cell>
-          <cell r="F122">
-            <v>1.969632</v>
-          </cell>
-        </row>
-        <row r="123">
-          <cell r="C123">
-            <v>6</v>
-          </cell>
-          <cell r="F123">
-            <v>1.7320990000000001</v>
-          </cell>
-        </row>
-        <row r="124">
-          <cell r="C124">
-            <v>7</v>
-          </cell>
-          <cell r="F124">
-            <v>1.7393719999999999</v>
-          </cell>
-        </row>
-        <row r="125">
-          <cell r="C125">
-            <v>8</v>
-          </cell>
-          <cell r="F125">
-            <v>2.1455799999999998</v>
-          </cell>
-        </row>
-        <row r="126">
-          <cell r="C126">
-            <v>9</v>
-          </cell>
-          <cell r="F126">
-            <v>2.1868280000000002</v>
-          </cell>
-        </row>
-        <row r="127">
-          <cell r="C127">
-            <v>10</v>
-          </cell>
-          <cell r="F127">
-            <v>2.1277750000000002</v>
-          </cell>
-        </row>
-        <row r="128">
-          <cell r="C128">
-            <v>2</v>
-          </cell>
-          <cell r="F128">
-            <v>1.6060559999999999</v>
-          </cell>
-        </row>
-        <row r="129">
-          <cell r="C129">
-            <v>3</v>
-          </cell>
-          <cell r="F129">
-            <v>2.0599120000000002</v>
-          </cell>
-        </row>
-        <row r="130">
-          <cell r="C130">
-            <v>4</v>
-          </cell>
-          <cell r="F130">
-            <v>2.4237299999999999</v>
-          </cell>
-        </row>
-        <row r="131">
-          <cell r="C131">
-            <v>5</v>
-          </cell>
-          <cell r="F131">
-            <v>1.9223779999999999</v>
-          </cell>
-        </row>
-        <row r="132">
-          <cell r="C132">
-            <v>6</v>
-          </cell>
-          <cell r="F132">
-            <v>1.7008639999999999</v>
-          </cell>
-        </row>
-        <row r="133">
-          <cell r="C133">
-            <v>7</v>
-          </cell>
-          <cell r="F133">
-            <v>1.679556</v>
-          </cell>
-        </row>
-        <row r="134">
-          <cell r="C134">
-            <v>8</v>
-          </cell>
-          <cell r="F134">
-            <v>2.1317870000000001</v>
-          </cell>
-        </row>
-        <row r="135">
-          <cell r="C135">
-            <v>9</v>
-          </cell>
-          <cell r="F135">
-            <v>2.2090960000000002</v>
-          </cell>
-        </row>
-        <row r="136">
-          <cell r="C136">
-            <v>10</v>
-          </cell>
-          <cell r="F136">
-            <v>2.375267</v>
-          </cell>
-        </row>
-        <row r="137">
-          <cell r="C137">
-            <v>2</v>
-          </cell>
-          <cell r="F137">
-            <v>1.6480939999999999</v>
-          </cell>
-        </row>
-        <row r="138">
-          <cell r="C138">
-            <v>3</v>
-          </cell>
-          <cell r="F138">
-            <v>2.3658739999999998</v>
-          </cell>
-        </row>
-        <row r="139">
-          <cell r="C139">
-            <v>4</v>
-          </cell>
-          <cell r="F139">
-            <v>2.564289</v>
-          </cell>
-        </row>
-        <row r="140">
-          <cell r="C140">
-            <v>5</v>
-          </cell>
-          <cell r="F140">
-            <v>2.3665099999999999</v>
-          </cell>
-        </row>
-        <row r="141">
-          <cell r="C141">
-            <v>6</v>
-          </cell>
-          <cell r="F141">
-            <v>2.5408569999999999</v>
-          </cell>
-        </row>
-        <row r="142">
-          <cell r="C142">
-            <v>7</v>
-          </cell>
-          <cell r="F142">
-            <v>2.594579</v>
-          </cell>
-        </row>
-        <row r="143">
-          <cell r="C143">
-            <v>8</v>
-          </cell>
-          <cell r="F143">
-            <v>2.7809370000000002</v>
-          </cell>
-        </row>
-        <row r="144">
-          <cell r="C144">
-            <v>9</v>
-          </cell>
-          <cell r="F144">
-            <v>2.3792759999999999</v>
-          </cell>
-        </row>
-        <row r="145">
-          <cell r="C145">
-            <v>10</v>
-          </cell>
-          <cell r="F145">
-            <v>2.6882269999999999</v>
-          </cell>
-        </row>
-        <row r="146">
-          <cell r="C146">
-            <v>2</v>
-          </cell>
-          <cell r="F146">
-            <v>1.6795</v>
-          </cell>
-        </row>
-        <row r="147">
-          <cell r="C147">
-            <v>3</v>
-          </cell>
-          <cell r="F147">
-            <v>2.200027</v>
-          </cell>
-        </row>
-        <row r="148">
-          <cell r="C148">
-            <v>4</v>
-          </cell>
-          <cell r="F148">
-            <v>2.6564809999999999</v>
-          </cell>
-        </row>
-        <row r="149">
-          <cell r="C149">
-            <v>5</v>
-          </cell>
-          <cell r="F149">
-            <v>2.471295</v>
-          </cell>
-        </row>
-        <row r="150">
-          <cell r="C150">
-            <v>6</v>
-          </cell>
-          <cell r="F150">
-            <v>2.6432600000000002</v>
-          </cell>
-        </row>
-        <row r="151">
-          <cell r="C151">
-            <v>7</v>
-          </cell>
-          <cell r="F151">
-            <v>2.7682220000000002</v>
-          </cell>
-        </row>
-        <row r="152">
-          <cell r="C152">
-            <v>8</v>
-          </cell>
-          <cell r="F152">
-            <v>2.636749</v>
-          </cell>
-        </row>
-        <row r="153">
-          <cell r="C153">
-            <v>9</v>
-          </cell>
-          <cell r="F153">
-            <v>2.8610639999999998</v>
-          </cell>
-        </row>
-        <row r="154">
-          <cell r="C154">
-            <v>10</v>
-          </cell>
-          <cell r="F154">
-            <v>2.905421</v>
-          </cell>
-        </row>
-        <row r="155">
-          <cell r="C155">
-            <v>2</v>
-          </cell>
-          <cell r="F155">
-            <v>1.6727190000000001</v>
-          </cell>
-        </row>
-        <row r="156">
-          <cell r="C156">
-            <v>3</v>
-          </cell>
-          <cell r="F156">
-            <v>2.2964009999999999</v>
-          </cell>
-        </row>
-        <row r="157">
-          <cell r="C157">
-            <v>4</v>
-          </cell>
-          <cell r="F157">
-            <v>2.7937069999999999</v>
-          </cell>
-        </row>
-        <row r="158">
-          <cell r="C158">
-            <v>5</v>
-          </cell>
-          <cell r="F158">
-            <v>2.5753460000000001</v>
-          </cell>
-        </row>
-        <row r="159">
-          <cell r="C159">
-            <v>6</v>
-          </cell>
-          <cell r="F159">
-            <v>2.7123919999999999</v>
-          </cell>
-        </row>
-        <row r="160">
-          <cell r="C160">
-            <v>7</v>
-          </cell>
-          <cell r="F160">
-            <v>2.8378549999999998</v>
-          </cell>
-        </row>
-        <row r="161">
-          <cell r="C161">
-            <v>8</v>
-          </cell>
-          <cell r="F161">
-            <v>3.0341049999999998</v>
-          </cell>
-        </row>
-        <row r="162">
-          <cell r="C162">
-            <v>9</v>
-          </cell>
-          <cell r="F162">
-            <v>3.0507810000000002</v>
-          </cell>
-        </row>
-        <row r="163">
-          <cell r="C163">
-            <v>10</v>
-          </cell>
-          <cell r="F163">
-            <v>3.0383200000000001</v>
-          </cell>
-        </row>
-        <row r="164">
-          <cell r="C164">
-            <v>2</v>
-          </cell>
-          <cell r="F164">
-            <v>1.6293329999999999</v>
-          </cell>
-        </row>
-        <row r="165">
-          <cell r="C165">
-            <v>3</v>
-          </cell>
-          <cell r="F165">
-            <v>2.2975289999999999</v>
-          </cell>
-        </row>
-        <row r="166">
-          <cell r="C166">
-            <v>4</v>
-          </cell>
-          <cell r="F166">
-            <v>2.2389860000000001</v>
-          </cell>
-        </row>
-        <row r="167">
-          <cell r="C167">
-            <v>5</v>
-          </cell>
-          <cell r="F167">
-            <v>2.5315699999999999</v>
-          </cell>
-        </row>
-        <row r="168">
-          <cell r="C168">
-            <v>6</v>
-          </cell>
-          <cell r="F168">
-            <v>2.7081189999999999</v>
-          </cell>
-        </row>
-        <row r="169">
-          <cell r="C169">
-            <v>7</v>
-          </cell>
-          <cell r="F169">
-            <v>2.86558</v>
-          </cell>
-        </row>
-        <row r="170">
-          <cell r="C170">
-            <v>8</v>
-          </cell>
-          <cell r="F170">
-            <v>2.9882569999999999</v>
-          </cell>
-        </row>
-        <row r="171">
-          <cell r="C171">
-            <v>9</v>
-          </cell>
-          <cell r="F171">
-            <v>2.9605480000000002</v>
-          </cell>
-        </row>
-        <row r="172">
-          <cell r="C172">
-            <v>10</v>
-          </cell>
-          <cell r="F172">
-            <v>3.0417550000000002</v>
-          </cell>
-        </row>
-        <row r="173">
-          <cell r="C173">
-            <v>2</v>
-          </cell>
-          <cell r="F173">
-            <v>1.6355109999999999</v>
-          </cell>
-        </row>
-        <row r="174">
-          <cell r="C174">
-            <v>3</v>
-          </cell>
-          <cell r="F174">
-            <v>2.1205129999999999</v>
-          </cell>
-        </row>
-        <row r="175">
-          <cell r="C175">
-            <v>4</v>
-          </cell>
-          <cell r="F175">
-            <v>2.9631210000000001</v>
-          </cell>
-        </row>
-        <row r="176">
-          <cell r="C176">
-            <v>5</v>
-          </cell>
-          <cell r="F176">
-            <v>2.4625439999999998</v>
-          </cell>
-        </row>
-        <row r="177">
-          <cell r="C177">
-            <v>6</v>
-          </cell>
-          <cell r="F177">
-            <v>2.6423480000000001</v>
-          </cell>
-        </row>
-        <row r="178">
-          <cell r="C178">
-            <v>7</v>
-          </cell>
-          <cell r="F178">
-            <v>2.765876</v>
-          </cell>
-        </row>
-        <row r="179">
-          <cell r="C179">
-            <v>8</v>
-          </cell>
-          <cell r="F179">
-            <v>2.9612989999999999</v>
-          </cell>
-        </row>
-        <row r="180">
-          <cell r="C180">
-            <v>9</v>
-          </cell>
-          <cell r="F180">
-            <v>2.8841299999999999</v>
-          </cell>
-        </row>
-        <row r="181">
-          <cell r="C181">
-            <v>10</v>
-          </cell>
-          <cell r="F181">
-            <v>2.7498040000000001</v>
-          </cell>
-        </row>
-        <row r="182">
-          <cell r="C182">
-            <v>2</v>
-          </cell>
-          <cell r="F182">
-            <v>1.8219810000000001</v>
-          </cell>
-        </row>
-        <row r="183">
-          <cell r="C183">
-            <v>3</v>
-          </cell>
-          <cell r="F183">
-            <v>2.7355119999999999</v>
-          </cell>
-        </row>
-        <row r="184">
-          <cell r="C184">
-            <v>4</v>
-          </cell>
-          <cell r="F184">
-            <v>3.2678989999999999</v>
-          </cell>
-        </row>
-        <row r="185">
-          <cell r="C185">
-            <v>5</v>
-          </cell>
-          <cell r="F185">
-            <v>3.3698060000000001</v>
-          </cell>
-        </row>
-        <row r="186">
-          <cell r="C186">
-            <v>6</v>
-          </cell>
-          <cell r="F186">
-            <v>3.64174</v>
-          </cell>
-        </row>
-        <row r="187">
-          <cell r="C187">
-            <v>7</v>
-          </cell>
-          <cell r="F187">
-            <v>3.8659889999999999</v>
-          </cell>
-        </row>
-        <row r="188">
-          <cell r="C188">
-            <v>8</v>
-          </cell>
-          <cell r="F188">
-            <v>4.1325240000000001</v>
-          </cell>
-        </row>
-        <row r="189">
-          <cell r="C189">
-            <v>9</v>
-          </cell>
-          <cell r="F189">
-            <v>4.4879239999999996</v>
-          </cell>
-        </row>
-        <row r="190">
-          <cell r="C190">
-            <v>10</v>
-          </cell>
-          <cell r="F190">
-            <v>4.3960889999999999</v>
-          </cell>
-        </row>
-        <row r="191">
-          <cell r="C191">
-            <v>2</v>
-          </cell>
-          <cell r="F191">
-            <v>1.8872150000000001</v>
-          </cell>
-        </row>
-        <row r="192">
-          <cell r="C192">
-            <v>3</v>
-          </cell>
-          <cell r="F192">
-            <v>2.703446</v>
-          </cell>
-        </row>
-        <row r="193">
-          <cell r="C193">
-            <v>4</v>
-          </cell>
-          <cell r="F193">
-            <v>3.3026990000000001</v>
-          </cell>
-        </row>
-        <row r="194">
-          <cell r="C194">
-            <v>5</v>
-          </cell>
-          <cell r="F194">
-            <v>3.3457560000000002</v>
-          </cell>
-        </row>
-        <row r="195">
-          <cell r="C195">
-            <v>6</v>
-          </cell>
-          <cell r="F195">
-            <v>3.7529240000000001</v>
-          </cell>
-        </row>
-        <row r="196">
-          <cell r="C196">
-            <v>7</v>
-          </cell>
-          <cell r="F196">
-            <v>4.0109469999999998</v>
-          </cell>
-        </row>
-        <row r="197">
-          <cell r="C197">
-            <v>8</v>
-          </cell>
-          <cell r="F197">
-            <v>4.3684669999999999</v>
-          </cell>
-        </row>
-        <row r="198">
-          <cell r="C198">
-            <v>9</v>
-          </cell>
-          <cell r="F198">
-            <v>4.4984999999999999</v>
-          </cell>
-        </row>
-        <row r="199">
-          <cell r="C199">
-            <v>10</v>
-          </cell>
-          <cell r="F199">
-            <v>4.5610239999999997</v>
-          </cell>
-        </row>
-        <row r="200">
-          <cell r="C200">
-            <v>2</v>
-          </cell>
-          <cell r="F200">
-            <v>1.919009</v>
-          </cell>
-        </row>
-        <row r="201">
-          <cell r="C201">
-            <v>3</v>
-          </cell>
-          <cell r="F201">
-            <v>2.7480419999999999</v>
-          </cell>
-        </row>
-        <row r="202">
-          <cell r="C202">
-            <v>4</v>
-          </cell>
-          <cell r="F202">
-            <v>3.2578659999999999</v>
-          </cell>
-        </row>
-        <row r="203">
-          <cell r="C203">
-            <v>5</v>
-          </cell>
-          <cell r="F203">
-            <v>3.141149</v>
-          </cell>
-        </row>
-        <row r="204">
-          <cell r="C204">
-            <v>6</v>
-          </cell>
-          <cell r="F204">
-            <v>3.5633180000000002</v>
-          </cell>
-        </row>
-        <row r="205">
-          <cell r="C205">
-            <v>7</v>
-          </cell>
-          <cell r="F205">
-            <v>3.9828999999999999</v>
-          </cell>
-        </row>
-        <row r="206">
-          <cell r="C206">
-            <v>8</v>
-          </cell>
-          <cell r="F206">
-            <v>4.1312860000000002</v>
-          </cell>
-        </row>
-        <row r="207">
-          <cell r="C207">
-            <v>9</v>
-          </cell>
-          <cell r="F207">
-            <v>4.4463549999999996</v>
-          </cell>
-        </row>
-        <row r="208">
-          <cell r="C208">
-            <v>10</v>
-          </cell>
-          <cell r="F208">
-            <v>4.5704099999999999</v>
-          </cell>
-        </row>
-        <row r="209">
-          <cell r="C209">
-            <v>2</v>
-          </cell>
-          <cell r="F209">
-            <v>1.8843859999999999</v>
-          </cell>
-        </row>
-        <row r="210">
-          <cell r="C210">
-            <v>3</v>
-          </cell>
-          <cell r="F210">
-            <v>2.6536970000000002</v>
-          </cell>
-        </row>
-        <row r="211">
-          <cell r="C211">
-            <v>4</v>
-          </cell>
-          <cell r="F211">
-            <v>2.7387350000000001</v>
-          </cell>
-        </row>
-        <row r="212">
-          <cell r="C212">
-            <v>5</v>
-          </cell>
-          <cell r="F212">
-            <v>3.2721149999999999</v>
-          </cell>
-        </row>
-        <row r="213">
-          <cell r="C213">
-            <v>6</v>
-          </cell>
-          <cell r="F213">
-            <v>3.5700989999999999</v>
-          </cell>
-        </row>
-        <row r="214">
-          <cell r="C214">
-            <v>7</v>
-          </cell>
-          <cell r="F214">
-            <v>3.914304</v>
-          </cell>
-        </row>
-        <row r="215">
-          <cell r="C215">
-            <v>8</v>
-          </cell>
-          <cell r="F215">
-            <v>4.1857139999999999</v>
-          </cell>
-        </row>
-        <row r="216">
-          <cell r="C216">
-            <v>9</v>
-          </cell>
-          <cell r="F216">
-            <v>4.5100920000000002</v>
-          </cell>
-        </row>
-        <row r="217">
-          <cell r="C217">
-            <v>10</v>
-          </cell>
-          <cell r="F217">
-            <v>4.5428620000000004</v>
-          </cell>
-        </row>
-        <row r="218">
-          <cell r="C218">
-            <v>2</v>
-          </cell>
-          <cell r="F218">
-            <v>1.817528</v>
-          </cell>
-        </row>
-        <row r="219">
-          <cell r="C219">
-            <v>3</v>
-          </cell>
-          <cell r="F219">
-            <v>2.7215159999999998</v>
-          </cell>
-        </row>
-        <row r="220">
-          <cell r="C220">
-            <v>4</v>
-          </cell>
-          <cell r="F220">
-            <v>3.3977400000000002</v>
-          </cell>
-        </row>
-        <row r="221">
-          <cell r="C221">
-            <v>5</v>
-          </cell>
-          <cell r="F221">
-            <v>3.1022669999999999</v>
-          </cell>
-        </row>
-        <row r="222">
-          <cell r="C222">
-            <v>6</v>
-          </cell>
-          <cell r="F222">
-            <v>3.5263629999999999</v>
-          </cell>
-        </row>
-        <row r="223">
-          <cell r="C223">
-            <v>7</v>
-          </cell>
-          <cell r="F223">
-            <v>3.788392</v>
-          </cell>
-        </row>
-        <row r="224">
-          <cell r="C224">
-            <v>8</v>
-          </cell>
-          <cell r="F224">
-            <v>4.0775300000000003</v>
-          </cell>
-        </row>
-        <row r="225">
-          <cell r="C225">
-            <v>9</v>
-          </cell>
-          <cell r="F225">
-            <v>3.8476210000000002</v>
-          </cell>
-        </row>
-        <row r="226">
-          <cell r="C226">
-            <v>10</v>
-          </cell>
-          <cell r="F226">
-            <v>4.6891160000000003</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_2" connectionId="6" xr16:uid="{1942F716-F614-4758-9060-DFDF761D6648}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="16" unboundColumnsRight="6">
@@ -10890,7 +9053,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="AC15" sqref="AC15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>